<commit_message>
modified for style and showing slider values
</commit_message>
<xml_diff>
--- a/interpretationTask/interpretationTaskConditions.xlsx
+++ b/interpretationTask/interpretationTaskConditions.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21901"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\que_d\Documents\McGill\LepageLab\psychopyExperiment_github\interpretationTask\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF9F985B-36A4-477C-AD18-36EC4F16CF8A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="12735" yWindow="2655" windowWidth="16065" windowHeight="12120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,12 +24,431 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="136">
+  <si>
+    <t>set</t>
+  </si>
+  <si>
+    <t>state1</t>
+  </si>
+  <si>
+    <t>state2</t>
+  </si>
+  <si>
+    <t>state3</t>
+  </si>
+  <si>
+    <t>sliderState1</t>
+  </si>
+  <si>
+    <t>sliderState2</t>
+  </si>
+  <si>
+    <t>sliderState3</t>
+  </si>
+  <si>
+    <t>sliderState4</t>
+  </si>
+  <si>
+    <t>set1</t>
+  </si>
+  <si>
+    <t>set2</t>
+  </si>
+  <si>
+    <t>set3</t>
+  </si>
+  <si>
+    <t>set4</t>
+  </si>
+  <si>
+    <t>set5</t>
+  </si>
+  <si>
+    <t>set6</t>
+  </si>
+  <si>
+    <t>set7</t>
+  </si>
+  <si>
+    <t>set8</t>
+  </si>
+  <si>
+    <t>set9</t>
+  </si>
+  <si>
+    <t>set10</t>
+  </si>
+  <si>
+    <t>set11</t>
+  </si>
+  <si>
+    <t>set12</t>
+  </si>
+  <si>
+    <t>set13</t>
+  </si>
+  <si>
+    <t>set14</t>
+  </si>
+  <si>
+    <t>set15</t>
+  </si>
+  <si>
+    <t>set16</t>
+  </si>
+  <si>
+    <t>Natasha ne sait pas qu'elle parle à sa mère.</t>
+  </si>
+  <si>
+    <t>Natasha est confuse et désorientée.</t>
+  </si>
+  <si>
+    <t>Natasha n'a pas mis son casque lorsqu'elle a fait du vélo.</t>
+  </si>
+  <si>
+    <t>Natasha est à une fête costumée pour l'Halloween.</t>
+  </si>
+  <si>
+    <t>Natasha vient tout juste d'apprendre qu'elle a été adoptée.</t>
+  </si>
+  <si>
+    <t>Natasha est très gênée.</t>
+  </si>
+  <si>
+    <t>Natasha a perdu la mémoire après avoir été frappée par une voiture.</t>
+  </si>
+  <si>
+    <t>Andrea s'est fait de nouveaux amis.</t>
+  </si>
+  <si>
+    <t>Les nouveaux amis d'Andrea contrôlent tous les aspects de sa vie.</t>
+  </si>
+  <si>
+    <t>Andrea a soudainement coupé tout contact avec sa famille.</t>
+  </si>
+  <si>
+    <t>Andrea vient tout juste de commencer à aller à l'université.</t>
+  </si>
+  <si>
+    <t>Andrea est une personne gentille et attentionnée.</t>
+  </si>
+  <si>
+    <t>Andrea aime être photographiée.</t>
+  </si>
+  <si>
+    <t>Andrea a joint une secte.</t>
+  </si>
+  <si>
+    <t>Nicolas conduit sa voiture très vite.</t>
+  </si>
+  <si>
+    <t>Nicolas ne s'est pas arrêté au feu rouge</t>
+  </si>
+  <si>
+    <t>Nicolas a blessé une petite fille avec sa voiture.</t>
+  </si>
+  <si>
+    <t>Nicolas est en retard pour son travail.</t>
+  </si>
+  <si>
+    <t>La femme de Nicolas va accoucher.</t>
+  </si>
+  <si>
+    <t>Nicolas déteste aller prendre une marche</t>
+  </si>
+  <si>
+    <t>Nicolas a commis un délit de fuite.</t>
+  </si>
+  <si>
+    <t>Tom et Michel crient.</t>
+  </si>
+  <si>
+    <t>Tom et Michel ont la nausée.</t>
+  </si>
+  <si>
+    <t>Tom et Michel ont trop mange de barbe à papa aujourd'hui.</t>
+  </si>
+  <si>
+    <t>Tom et Michel sont à une partie de basketball.</t>
+  </si>
+  <si>
+    <t>Tom et Michel ont trouvé un corps mort dans la ruelle.</t>
+  </si>
+  <si>
+    <t>Tom et Michel apprécient être le centre d'intérêt.</t>
+  </si>
+  <si>
+    <t>Tom et Michel ont du plaisir dans les montagnes russes.</t>
+  </si>
+  <si>
+    <t>Jenny ne peut pas s'endormir.</t>
+  </si>
+  <si>
+    <t>Jenny est impatiente que le matin arrive enfin.</t>
+  </si>
+  <si>
+    <t>Jenny se demande combien il y aura de cadeaux sous le sapin.</t>
+  </si>
+  <si>
+    <t>Jenny est nerveuse à propos de ses examens le lendemain</t>
+  </si>
+  <si>
+    <t>Jenny est inquiète pour sa mère qui est malade.</t>
+  </si>
+  <si>
+    <t>Jenny aime son lit.</t>
+  </si>
+  <si>
+    <t>Jenny est excitée à l'idée du matin de Noël.</t>
+  </si>
+  <si>
+    <t>L'homme est un orateur public d'expérience.</t>
+  </si>
+  <si>
+    <t>Les mêmes personnes viennent écouter l'homme chaque semaine.</t>
+  </si>
+  <si>
+    <t>L'homme porte de longues robes.</t>
+  </si>
+  <si>
+    <t>L'homme est un politicien.</t>
+  </si>
+  <si>
+    <t>L'homme est un activiste pour les droits des gais.</t>
+  </si>
+  <si>
+    <t>L'homme est timide.</t>
+  </si>
+  <si>
+    <t>L'homme est un prêtre</t>
+  </si>
+  <si>
+    <t>Richard porte parfois du maquillage.</t>
+  </si>
+  <si>
+    <t>Richard passe la majorité de son temps au théâtre.</t>
+  </si>
+  <si>
+    <t>Richard est allé à l'école de théâtre.</t>
+  </si>
+  <si>
+    <t>Richard est un travesti.</t>
+  </si>
+  <si>
+    <t>Richard est préoccupé par ses cicatrices.</t>
+  </si>
+  <si>
+    <t>Richard souhaiterait avoir une femme.</t>
+  </si>
+  <si>
+    <t>Richard est un comédien.</t>
+  </si>
+  <si>
+    <t>Stella répond au téléphone à son travail.</t>
+  </si>
+  <si>
+    <t>Stella est une femme puissante.</t>
+  </si>
+  <si>
+    <t>Stella est allée à l'école de Droit.</t>
+  </si>
+  <si>
+    <t>Stella est une secrétaire.</t>
+  </si>
+  <si>
+    <t>Stella est une opératrice du 911.</t>
+  </si>
+  <si>
+    <t>Stella est une gardienne.</t>
+  </si>
+  <si>
+    <t>Stella est avocate.</t>
+  </si>
+  <si>
+    <t>Étienne est surpris.</t>
+  </si>
+  <si>
+    <t>La valise d'Étienne est faite.</t>
+  </si>
+  <si>
+    <t>Étienne est très malade et ne peut plus vivre à la maison.</t>
+  </si>
+  <si>
+    <t>L'épouse d'Étienne l'emmène en vacances.</t>
+  </si>
+  <si>
+    <t>Étienne s'est fait expulser parce qu'il faisait trop de party</t>
+  </si>
+  <si>
+    <t>Étienne dort à poings fermés</t>
+  </si>
+  <si>
+    <t>Étienne a besoin qu'on le soigne</t>
+  </si>
+  <si>
+    <t>Daniel est très chanceux.</t>
+  </si>
+  <si>
+    <t>Daniel a toujours souhaité que ça arrive.</t>
+  </si>
+  <si>
+    <t>Daniel va toujours se souvenir du jour où il l’a demandée en mariage.</t>
+  </si>
+  <si>
+    <t>Daniel a eu des billets pour voir son groupe favori.</t>
+  </si>
+  <si>
+    <t>Daniel vient de gagner à la loterie.</t>
+  </si>
+  <si>
+    <t>Daniel a glissé sur une peau de banane.</t>
+  </si>
+  <si>
+    <t>Daniel s’est marié.</t>
+  </si>
+  <si>
+    <t>Fred a obtenu une note très forte à son examen.</t>
+  </si>
+  <si>
+    <t>Il n’est habituellement pas très doué à l’école.</t>
+  </si>
+  <si>
+    <t>Le professeur l’a pris à copier sur un autre étudiant.</t>
+  </si>
+  <si>
+    <t>Fred est un étudiant qui travaille fort.</t>
+  </si>
+  <si>
+    <t>Fred est vraiment intelligent.</t>
+  </si>
+  <si>
+    <t>Fred est une grenouille.</t>
+  </si>
+  <si>
+    <t>Fred est très malhonnête.</t>
+  </si>
+  <si>
+    <t>Amy incite les enfants à faire de l'exercice.</t>
+  </si>
+  <si>
+    <t>Amy est très protectrice envers les enfants.</t>
+  </si>
+  <si>
+    <t>À la maison, Amy jappe bruyamment lorsqu'on sonne à la porte.</t>
+  </si>
+  <si>
+    <t>Amy est professeure d'éducation physique.</t>
+  </si>
+  <si>
+    <t>Amy est une mère très active.</t>
+  </si>
+  <si>
+    <t>Amy is not a very caring person.</t>
+  </si>
+  <si>
+    <t>Amy est un chien.</t>
+  </si>
+  <si>
+    <t>Stéphane est à genoux.</t>
+  </si>
+  <si>
+    <t>Stéphane pleure.</t>
+  </si>
+  <si>
+    <t>La femme de Stéphane a fait ses bagages.</t>
+  </si>
+  <si>
+    <t>Stéphane prie.</t>
+  </si>
+  <si>
+    <t>Stéphane s'apprête à demander sa fiancée en mariage.</t>
+  </si>
+  <si>
+    <t>Stéphane souhaiterait être un nain magique.</t>
+  </si>
+  <si>
+    <t>Stéphane n'arrive pas à trouver sa sacoche.</t>
+  </si>
+  <si>
+    <t>Joanne n’entre plus dans ses vêtements d’été.</t>
+  </si>
+  <si>
+    <t>La famille de Joanne veut l’aider.</t>
+  </si>
+  <si>
+    <t>Joanne a vraiment hâte de voir son nouveau bébé.</t>
+  </si>
+  <si>
+    <t>Joanne va aller s’acheter une nouvelle garde-robe.</t>
+  </si>
+  <si>
+    <t>Joanne désire perdre du poids.</t>
+  </si>
+  <si>
+    <t>La température hivernale fait rapetisser Joanne.</t>
+  </si>
+  <si>
+    <t>Joanne est enceinte.</t>
+  </si>
+  <si>
+    <t>Alice est impatiente de prendre l’autobus.</t>
+  </si>
+  <si>
+    <t>Alice n’a pas eu le temps de faire ses bagages.</t>
+  </si>
+  <si>
+    <t>Alice a vraiment peur de son cruel beau père.</t>
+  </si>
+  <si>
+    <t>Alice va en vacances.</t>
+  </si>
+  <si>
+    <t>Alice s’en va à un collège loin de chez elle.</t>
+  </si>
+  <si>
+    <t>Alice aime envoyer la main aux gens.</t>
+  </si>
+  <si>
+    <t>Alice se sauve de chez elle.</t>
+  </si>
+  <si>
+    <t>Jean est un homme d'affaires prospère.</t>
+  </si>
+  <si>
+    <t>Les clients de Jean sont surtout de jeunes hommes.</t>
+  </si>
+  <si>
+    <t>Jean ne se fait jamais prendre par la police.</t>
+  </si>
+  <si>
+    <t>Jean est un gérant de banque.</t>
+  </si>
+  <si>
+    <t>Jean est propriétaire d'un centre de réhabilitation.</t>
+  </si>
+  <si>
+    <t>Jean est un proxénète.</t>
+  </si>
+  <si>
+    <t>Jean est un vendeur de drogue.</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -49,8 +474,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -330,13 +758,460 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E3" t="s">
+        <v>34</v>
+      </c>
+      <c r="F3" t="s">
+        <v>35</v>
+      </c>
+      <c r="G3" t="s">
+        <v>36</v>
+      </c>
+      <c r="H3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E4" t="s">
+        <v>41</v>
+      </c>
+      <c r="F4" t="s">
+        <v>42</v>
+      </c>
+      <c r="G4" t="s">
+        <v>43</v>
+      </c>
+      <c r="H4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D5" t="s">
+        <v>47</v>
+      </c>
+      <c r="E5" t="s">
+        <v>48</v>
+      </c>
+      <c r="F5" t="s">
+        <v>49</v>
+      </c>
+      <c r="G5" t="s">
+        <v>50</v>
+      </c>
+      <c r="H5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D6" t="s">
+        <v>54</v>
+      </c>
+      <c r="E6" t="s">
+        <v>55</v>
+      </c>
+      <c r="F6" t="s">
+        <v>56</v>
+      </c>
+      <c r="G6" t="s">
+        <v>57</v>
+      </c>
+      <c r="H6" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s">
+        <v>59</v>
+      </c>
+      <c r="C7" t="s">
+        <v>60</v>
+      </c>
+      <c r="D7" t="s">
+        <v>61</v>
+      </c>
+      <c r="E7" t="s">
+        <v>62</v>
+      </c>
+      <c r="F7" t="s">
+        <v>63</v>
+      </c>
+      <c r="G7" t="s">
+        <v>64</v>
+      </c>
+      <c r="H7" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" t="s">
+        <v>66</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D8" t="s">
+        <v>68</v>
+      </c>
+      <c r="E8" t="s">
+        <v>69</v>
+      </c>
+      <c r="F8" t="s">
+        <v>70</v>
+      </c>
+      <c r="G8" t="s">
+        <v>71</v>
+      </c>
+      <c r="H8" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" t="s">
+        <v>73</v>
+      </c>
+      <c r="C9" t="s">
+        <v>74</v>
+      </c>
+      <c r="D9" t="s">
+        <v>75</v>
+      </c>
+      <c r="E9" t="s">
+        <v>76</v>
+      </c>
+      <c r="F9" t="s">
+        <v>77</v>
+      </c>
+      <c r="G9" t="s">
+        <v>78</v>
+      </c>
+      <c r="H9" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" t="s">
+        <v>80</v>
+      </c>
+      <c r="C10" t="s">
+        <v>81</v>
+      </c>
+      <c r="D10" t="s">
+        <v>82</v>
+      </c>
+      <c r="E10" t="s">
+        <v>83</v>
+      </c>
+      <c r="F10" t="s">
+        <v>84</v>
+      </c>
+      <c r="G10" t="s">
+        <v>85</v>
+      </c>
+      <c r="H10" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" t="s">
+        <v>87</v>
+      </c>
+      <c r="C11" t="s">
+        <v>88</v>
+      </c>
+      <c r="D11" t="s">
+        <v>89</v>
+      </c>
+      <c r="E11" t="s">
+        <v>90</v>
+      </c>
+      <c r="F11" t="s">
+        <v>91</v>
+      </c>
+      <c r="G11" t="s">
+        <v>92</v>
+      </c>
+      <c r="H11" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" t="s">
+        <v>94</v>
+      </c>
+      <c r="C12" t="s">
+        <v>95</v>
+      </c>
+      <c r="D12" t="s">
+        <v>96</v>
+      </c>
+      <c r="E12" t="s">
+        <v>97</v>
+      </c>
+      <c r="F12" t="s">
+        <v>98</v>
+      </c>
+      <c r="G12" t="s">
+        <v>99</v>
+      </c>
+      <c r="H12" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" t="s">
+        <v>101</v>
+      </c>
+      <c r="C13" t="s">
+        <v>102</v>
+      </c>
+      <c r="D13" t="s">
+        <v>103</v>
+      </c>
+      <c r="E13" t="s">
+        <v>104</v>
+      </c>
+      <c r="F13" t="s">
+        <v>105</v>
+      </c>
+      <c r="G13" t="s">
+        <v>106</v>
+      </c>
+      <c r="H13" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" t="s">
+        <v>108</v>
+      </c>
+      <c r="C14" t="s">
+        <v>109</v>
+      </c>
+      <c r="D14" t="s">
+        <v>110</v>
+      </c>
+      <c r="E14" t="s">
+        <v>111</v>
+      </c>
+      <c r="F14" t="s">
+        <v>112</v>
+      </c>
+      <c r="G14" t="s">
+        <v>113</v>
+      </c>
+      <c r="H14" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" t="s">
+        <v>115</v>
+      </c>
+      <c r="C15" t="s">
+        <v>116</v>
+      </c>
+      <c r="D15" t="s">
+        <v>117</v>
+      </c>
+      <c r="E15" t="s">
+        <v>118</v>
+      </c>
+      <c r="F15" t="s">
+        <v>119</v>
+      </c>
+      <c r="G15" t="s">
+        <v>120</v>
+      </c>
+      <c r="H15" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" t="s">
+        <v>122</v>
+      </c>
+      <c r="C16" t="s">
+        <v>123</v>
+      </c>
+      <c r="D16" t="s">
+        <v>124</v>
+      </c>
+      <c r="E16" t="s">
+        <v>125</v>
+      </c>
+      <c r="F16" t="s">
+        <v>126</v>
+      </c>
+      <c r="G16" t="s">
+        <v>127</v>
+      </c>
+      <c r="H16" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" t="s">
+        <v>129</v>
+      </c>
+      <c r="C17" t="s">
+        <v>130</v>
+      </c>
+      <c r="D17" t="s">
+        <v>131</v>
+      </c>
+      <c r="E17" t="s">
+        <v>132</v>
+      </c>
+      <c r="F17" t="s">
+        <v>133</v>
+      </c>
+      <c r="G17" t="s">
+        <v>134</v>
+      </c>
+      <c r="H17" t="s">
+        <v>135</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>